<commit_message>
Script updated from Windows Laptop
</commit_message>
<xml_diff>
--- a/Basic Programs/Python Exercise Important Notes.xlsx
+++ b/Basic Programs/Python Exercise Important Notes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cisco-my.sharepoint.com/personal/merhassa_cisco_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cisco-my.sharepoint.com/personal/merhassa_cisco_com/Documents/Desktop/GIT REPO/Basic Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC104826899E7BA25ADE5928" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3492EA3-35AB-498B-8A8F-70DF14C59CA8}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_F25DC773A252ABDACC104826899E7BA25ADE5928" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0425DD9-B16E-450D-A954-B36FC835434C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>S.No</t>
   </si>
@@ -71,13 +71,25 @@
   </si>
   <si>
     <t>Exercise - Create list.py</t>
+  </si>
+  <si>
+    <t>Use join() and split()</t>
+  </si>
+  <si>
+    <t>Exercise - Check if number is prime</t>
+  </si>
+  <si>
+    <t>Exercise: DNA sequencing</t>
+  </si>
+  <si>
+    <t>Convert digit except ACTG to ' ' --&gt; join --&gt; Split --&gt; Sort Reverse wrt len</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +105,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -147,6 +171,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +456,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,7 +465,7 @@
     <col min="2" max="2" width="48.54296875" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="57" customWidth="1"/>
+    <col min="5" max="5" width="60.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -503,26 +529,44 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">

</xml_diff>

<commit_message>
Script Updated Windows Laptop
</commit_message>
<xml_diff>
--- a/Basic Programs/Python Exercise Important Notes.xlsx
+++ b/Basic Programs/Python Exercise Important Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cisco-my.sharepoint.com/personal/merhassa_cisco_com/Documents/Desktop/GIT REPO/Basic Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="11_F25DC773A252ABDACC104826899E7BA25ADE5928" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A419FB7C-D22D-40EE-BEF7-EA5CCF9377B3}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="11_F25DC773A252ABDACC104826899E7BA25ADE5928" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5221CCF-4781-4878-9530-5F8328DC1466}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -268,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +290,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -356,6 +362,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1703,7 +1718,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1717,7 +1732,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="15">
-        <f t="shared" ref="A1:D1" si="0">COUNTA(B3:B36)</f>
+        <f t="shared" ref="B1" si="0">COUNTA(B3:B36)</f>
         <v>34</v>
       </c>
       <c r="C1" s="15">
@@ -1941,17 +1956,17 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="11">
+    <row r="19" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="16">
         <v>17</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="11"/>
+      <c r="C19" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="11">

</xml_diff>